<commit_message>
project done for now
</commit_message>
<xml_diff>
--- a/output/freelance_gigs.xlsx
+++ b/output/freelance_gigs.xlsx
@@ -9,9 +9,7 @@
   <sheets>
     <sheet name="Freelance Gigs" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Freelance Gigs'!$A$1:$I$1</definedName>
-  </definedNames>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -19,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -32,12 +30,8 @@
       <color rgb="00FFFFFF"/>
       <sz val="11"/>
     </font>
-    <font>
-      <color rgb="000563C1"/>
-      <u val="single"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -62,8 +56,14 @@
         <bgColor rgb="00FFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC7CE"/>
+        <bgColor rgb="00FFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -71,27 +71,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -457,7 +455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -471,9 +469,9 @@
     <col width="20" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="8" customWidth="1" min="6" max="6"/>
-    <col width="50" customWidth="1" min="7" max="7"/>
-    <col width="60" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="40" customWidth="1" min="7" max="7"/>
+    <col width="50" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
@@ -505,7 +503,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Score</t>
+          <t>AI Score</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -527,12 +525,12 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Software Developer AI Trainer, $100-$130/hour</t>
+          <t>Web Developer | Remote</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>LinkedIn</t>
+          <t>Crossing Hurdles</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
@@ -547,7 +545,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F2" s="3" t="n">
@@ -555,34 +553,34 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Clear pay range, reputable company</t>
-        </is>
-      </c>
-      <c r="H2" s="4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/software-developer-ai-trainer-%24100-%24130-hour-at-linkedin-4368015576</t>
+          <t>Remote opportunity with a reputable company</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/web-developer-remote-at-crossing-hurdles-4360868838</t>
         </is>
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
-          <t>2026-02-04 15:43:28</t>
+          <t>2026-02-04 18:23:08</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Web Developer</t>
+          <t>Freelance Website Developer</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Engenium Inc</t>
+          <t>Bellweather Agency</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>Orlando, FL</t>
+          <t>New York, United States</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
@@ -592,42 +590,42 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
-        </is>
-      </c>
-      <c r="F3" s="5" t="n">
-        <v>5</v>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>7</v>
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Recent posting and clear job title</t>
-        </is>
-      </c>
-      <c r="H3" s="4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/web-developer-at-engenium-inc-4366186335</t>
+          <t>Freelance opportunity with a specific agency</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/freelance-website-developer-at-bellweather-agency-4368836167</t>
         </is>
       </c>
       <c r="I3" s="2" t="inlineStr">
         <is>
-          <t>2026-02-04 15:43:28</t>
+          <t>2026-02-04 18:23:08</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Web Developer</t>
+          <t>Creative Front End Developer (Freelance)</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>Gridiron IT</t>
+          <t>HAUS</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Washington, DC</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
@@ -637,32 +635,32 @@
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
-        </is>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>5</v>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>7</v>
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>Recent posting and clear company name</t>
-        </is>
-      </c>
-      <c r="H4" s="4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/web-developer-at-gridiron-it-4361261040</t>
+          <t>Creative freelance opportunity with a design-focused company</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/creative-front-end-developer-freelance-at-haus-4363858064</t>
         </is>
       </c>
       <c r="I4" s="2" t="inlineStr">
         <is>
-          <t>2026-02-04 15:43:28</t>
+          <t>2026-02-04 18:23:08</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Website Developer (Freelance)</t>
+          <t>Freelance Website Developer</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -682,42 +680,42 @@
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
-        </is>
-      </c>
-      <c r="F5" s="5" t="n">
-        <v>5</v>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>Recent posting and clear job title</t>
-        </is>
-      </c>
-      <c r="H5" s="4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/website-developer-freelance-at-twine-4352271108</t>
+          <t>Freelance opportunity with a platform that connects developers with clients</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/freelance-website-developer-at-twine-4352040027</t>
         </is>
       </c>
       <c r="I5" s="2" t="inlineStr">
         <is>
-          <t>2026-02-04 15:43:28</t>
+          <t>2026-02-04 18:23:08</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>Frontend Software Engineer | $120/hr Remote</t>
+          <t>Software Engineer</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>Crossing Hurdles</t>
+          <t>Astra</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Alameda, CA</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
@@ -727,42 +725,42 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
-        </is>
-      </c>
-      <c r="F6" s="5" t="n">
-        <v>6</v>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>9</v>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>Recent posting, clear job title, and competitive hourly rate</t>
-        </is>
-      </c>
-      <c r="H6" s="4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/frontend-software-engineer-%24120-hr-remote-at-crossing-hurdles-4360058864</t>
+          <t>Full-time software engineer position at a well-known company</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-engineer-at-astra-4246712185</t>
         </is>
       </c>
       <c r="I6" s="2" t="inlineStr">
         <is>
-          <t>2026-02-04 15:43:28</t>
+          <t>2026-02-04 18:23:08</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>Freelance Web Developer</t>
+          <t>Web Developer</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>Twine</t>
+          <t>Gridiron IT</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Washington, DC</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
@@ -772,42 +770,42 @@
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
-        </is>
-      </c>
-      <c r="F7" s="5" t="n">
-        <v>5</v>
+          <t>2026-01-12</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Recent posting and clear job title</t>
-        </is>
-      </c>
-      <c r="H7" s="4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/freelance-web-developer-at-twine-4354062554</t>
+          <t>Full-time web developer position in a major city</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/web-developer-at-gridiron-it-4361261040</t>
         </is>
       </c>
       <c r="I7" s="2" t="inlineStr">
         <is>
-          <t>2026-02-04 15:43:28</t>
+          <t>2026-02-04 18:23:08</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>React JS</t>
+          <t>Website Developer (Freelance)</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>Skybeyo</t>
+          <t>Twine</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>Bothell, WA</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
@@ -817,42 +815,42 @@
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
-        </is>
-      </c>
-      <c r="F8" s="5" t="n">
-        <v>5</v>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>7</v>
       </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
-          <t>Recent posting and clear job title</t>
-        </is>
-      </c>
-      <c r="H8" s="4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/react-js-at-skybeyo-4366039240</t>
+          <t>Freelance opportunity with a reputable platform</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/website-developer-freelance-at-twine-4352271108</t>
         </is>
       </c>
       <c r="I8" s="2" t="inlineStr">
         <is>
-          <t>2026-02-04 15:43:28</t>
+          <t>2026-02-04 18:23:08</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>Software Engineer | $90/hr Remote</t>
+          <t>Front-End Web Application Developer</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>Crossing Hurdles</t>
+          <t>PlanIT Group, LLC</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Alpharetta, GA</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
@@ -862,42 +860,42 @@
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2025-06-19</t>
         </is>
       </c>
       <c r="F9" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Clear pay rate, recent posting date</t>
-        </is>
-      </c>
-      <c r="H9" s="4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/software-engineer-%2490-hr-remote-at-crossing-hurdles-4359282892</t>
+          <t>Full-time position with a clear job title and location</t>
+        </is>
+      </c>
+      <c r="H9" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/front-end-web-application-developer-at-planit-group-llc-4251380445</t>
         </is>
       </c>
       <c r="I9" s="2" t="inlineStr">
         <is>
-          <t>2026-02-04 15:43:29</t>
+          <t>2026-02-04 18:23:08</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>Software Engineer - Python (Advanced)</t>
+          <t>Web Developer</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>Alignerr</t>
+          <t>CGR Creative</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Charlotte, NC</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
@@ -907,25 +905,25 @@
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
-        </is>
-      </c>
-      <c r="F10" s="5" t="n">
-        <v>5</v>
+          <t>2025-10-23</t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>7</v>
       </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
-          <t>Contract/freelance type and reputable location</t>
-        </is>
-      </c>
-      <c r="H10" s="4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/software-engineer-python-advanced-at-alignerr-4366244522</t>
+          <t>Full-time web development position with a creative company</t>
+        </is>
+      </c>
+      <c r="H10" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/web-developer-at-cgr-creative-4318750902</t>
         </is>
       </c>
       <c r="I10" s="2" t="inlineStr">
         <is>
-          <t>2026-02-04 15:43:29</t>
+          <t>2026-02-04 18:23:09</t>
         </is>
       </c>
     </row>
@@ -937,12 +935,12 @@
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>HeartCentrix Solutions</t>
+          <t>Engenium Inc</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>West Jordan, UT</t>
+          <t>Orlando, FL</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
@@ -952,37 +950,37 @@
       </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
-        </is>
-      </c>
-      <c r="F11" s="5" t="n">
-        <v>5</v>
+          <t>2026-01-26</t>
+        </is>
+      </c>
+      <c r="F11" s="4" t="n">
+        <v>7</v>
       </c>
       <c r="G11" s="2" t="inlineStr">
         <is>
-          <t>Contract/freelance type and specific location</t>
-        </is>
-      </c>
-      <c r="H11" s="4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/web-developer-at-heartcentrix-solutions-4356521567</t>
+          <t>Full-time web development position with a reputable company</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/web-developer-at-engenium-inc-4366186335</t>
         </is>
       </c>
       <c r="I11" s="2" t="inlineStr">
         <is>
-          <t>2026-02-04 15:43:29</t>
+          <t>2026-02-04 18:23:09</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>Application Engineer</t>
+          <t>Frontend Software Engineer | $120/hr Remote</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>Franklin Fitch</t>
+          <t>Crossing Hurdles</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
@@ -997,37 +995,37 @@
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
-        </is>
-      </c>
-      <c r="F12" s="5" t="n">
-        <v>5</v>
+          <t>2026-01-19</t>
+        </is>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>9</v>
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
-          <t>Contract/freelance type and reputable company</t>
-        </is>
-      </c>
-      <c r="H12" s="4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/application-engineer-at-franklin-fitch-4366611035</t>
+          <t>High-paying remote frontend software engineer position</t>
+        </is>
+      </c>
+      <c r="H12" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/frontend-software-engineer-%24120-hr-remote-at-crossing-hurdles-4360058864</t>
         </is>
       </c>
       <c r="I12" s="2" t="inlineStr">
         <is>
-          <t>2026-02-04 15:43:29</t>
+          <t>2026-02-04 18:23:09</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>Software Engineer | Remote</t>
+          <t>Freelance Web Developer</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>Crossing Hurdles</t>
+          <t>Twine</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr">
@@ -1042,42 +1040,42 @@
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
-        </is>
-      </c>
-      <c r="F13" s="5" t="n">
-        <v>5</v>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="F13" s="4" t="n">
+        <v>7</v>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Contract/freelance type, remote work, and recent posting</t>
-        </is>
-      </c>
-      <c r="H13" s="4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/software-engineer-remote-at-crossing-hurdles-4367885123</t>
+          <t>Freelance web development opportunity with a reputable platform</t>
+        </is>
+      </c>
+      <c r="H13" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/freelance-web-developer-at-twine-4354062554</t>
         </is>
       </c>
       <c r="I13" s="2" t="inlineStr">
         <is>
-          <t>2026-02-04 15:43:29</t>
+          <t>2026-02-04 18:23:09</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>Web Developer (Freelance)</t>
+          <t>React JS</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>Twine</t>
+          <t>Skybeyo</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Bothell, WA</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
@@ -1087,37 +1085,37 @@
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
-        </is>
-      </c>
-      <c r="F14" s="5" t="n">
-        <v>5</v>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="F14" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="G14" s="2" t="inlineStr">
         <is>
-          <t>Explicitly freelance and recent posting</t>
-        </is>
-      </c>
-      <c r="H14" s="4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/web-developer-freelance-at-twine-4357552100</t>
+          <t>React JS position with a company, but details are limited</t>
+        </is>
+      </c>
+      <c r="H14" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/react-js-at-skybeyo-4366039240</t>
         </is>
       </c>
       <c r="I14" s="2" t="inlineStr">
         <is>
-          <t>2026-02-04 15:43:29</t>
+          <t>2026-02-04 18:23:09</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>Software Engineer | $80/hr | Remote</t>
+          <t>Software Developer AI Trainer, $100-$130/hour</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>Crossing Hurdles</t>
+          <t>LinkedIn</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
@@ -1132,42 +1130,42 @@
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
-        </is>
-      </c>
-      <c r="F15" s="5" t="n">
-        <v>5</v>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>9</v>
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Clear pay rate, contract/freelance type</t>
-        </is>
-      </c>
-      <c r="H15" s="4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/software-engineer-%2480-hr-remote-at-crossing-hurdles-4332552298</t>
+          <t>High-paying software developer position with a reputable company like LinkedIn</t>
+        </is>
+      </c>
+      <c r="H15" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-developer-ai-trainer-%24100-%24130-hour-at-linkedin-4368015576</t>
         </is>
       </c>
       <c r="I15" s="2" t="inlineStr">
         <is>
-          <t>2026-02-04 15:43:30</t>
+          <t>2026-02-04 18:23:09</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>Freelance Web Developer – SaaS Remote</t>
+          <t>Front-End Developer (Local to TX)</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>Twine</t>
+          <t>SIDRAM TECHNOLOGIES</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Valley Spring, TX</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
@@ -1177,42 +1175,42 @@
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
-        </is>
-      </c>
-      <c r="F16" s="5" t="n">
-        <v>5</v>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="F16" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="G16" s="2" t="inlineStr">
         <is>
-          <t>Reputable company, clear job title</t>
-        </is>
-      </c>
-      <c r="H16" s="4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/freelance-web-developer-%E2%80%93-saas-remote-at-twine-4353884798</t>
+          <t>Full-time front-end development position, but location is limited to TX</t>
+        </is>
+      </c>
+      <c r="H16" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/front-end-developer-local-to-tx-at-sidram-technologies-4297653057</t>
         </is>
       </c>
       <c r="I16" s="2" t="inlineStr">
         <is>
-          <t>2026-02-04 15:43:30</t>
+          <t>2026-02-04 18:23:09</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>Software Engineer | $80/hr Remote</t>
+          <t>React Frontend Developer</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>Crossing Hurdles</t>
+          <t>Saransh Inc</t>
         </is>
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Bentonville, AR</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
@@ -1222,42 +1220,42 @@
       </c>
       <c r="E17" s="2" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
-        </is>
-      </c>
-      <c r="F17" s="5" t="n">
-        <v>6</v>
+          <t>2025-10-15</t>
+        </is>
+      </c>
+      <c r="F17" s="4" t="n">
+        <v>7</v>
       </c>
       <c r="G17" s="2" t="inlineStr">
         <is>
-          <t>Clear hourly rate, reputable company</t>
-        </is>
-      </c>
-      <c r="H17" s="4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/software-engineer-%2480-hr-remote-at-crossing-hurdles-4368230010</t>
+          <t>Full-time react frontend development position with a company</t>
+        </is>
+      </c>
+      <c r="H17" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/react-frontend-developer-at-saransh-inc-4315306148</t>
         </is>
       </c>
       <c r="I17" s="2" t="inlineStr">
         <is>
-          <t>2026-02-04 15:43:30</t>
+          <t>2026-02-04 18:23:09</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>Software Engineer, University Graduate</t>
+          <t>Tech. Strategy Developer (Junior)</t>
         </is>
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>HeyGen</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>Palo Alto, CA</t>
+          <t>Plano, TX</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
@@ -1267,42 +1265,42 @@
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
-        </is>
-      </c>
-      <c r="F18" s="5" t="n">
-        <v>5</v>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="F18" s="4" t="n">
+        <v>7</v>
       </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
-          <t>Reputable company, clear job title</t>
-        </is>
-      </c>
-      <c r="H18" s="4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/software-engineer-university-graduate-at-heygen-4355444896</t>
+          <t>Junior role with potential for growth</t>
+        </is>
+      </c>
+      <c r="H18" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/tech-strategy-developer-junior-at-op-4344464869</t>
         </is>
       </c>
       <c r="I18" s="2" t="inlineStr">
         <is>
-          <t>2026-02-04 15:43:30</t>
+          <t>2026-02-04 18:23:09</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>Software Engineer | Remote</t>
+          <t>Full Stack Engineer (TypeScript + Python)</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>Crossing Hurdles</t>
+          <t>Enexus Global Inc.</t>
         </is>
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Oakland, CA</t>
         </is>
       </c>
       <c r="D19" s="2" t="inlineStr">
@@ -1312,42 +1310,42 @@
       </c>
       <c r="E19" s="2" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
-        </is>
-      </c>
-      <c r="F19" s="5" t="n">
-        <v>5</v>
+          <t>2025-08-14</t>
+        </is>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="G19" s="2" t="inlineStr">
         <is>
-          <t>Reputable company, clear job title</t>
-        </is>
-      </c>
-      <c r="H19" s="4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/software-engineer-remote-at-crossing-hurdles-4368210715</t>
+          <t>Full stack role with good technologies and location</t>
+        </is>
+      </c>
+      <c r="H19" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/full-stack-engineer-typescript-%2B-python-at-enexus-global-inc-4285919998</t>
         </is>
       </c>
       <c r="I19" s="2" t="inlineStr">
         <is>
-          <t>2026-02-04 15:43:30</t>
+          <t>2026-02-04 18:23:09</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>Web Developer</t>
+          <t>Software Engineer</t>
         </is>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>BuzzClan</t>
+          <t>Incline</t>
         </is>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>Houston, TX</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="D20" s="2" t="inlineStr">
@@ -1357,97 +1355,1649 @@
       </c>
       <c r="E20" s="2" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
-        </is>
-      </c>
-      <c r="F20" s="5" t="n">
-        <v>5</v>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="F20" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="G20" s="2" t="inlineStr">
         <is>
-          <t>Reputable company, clear job title</t>
-        </is>
-      </c>
-      <c r="H20" s="4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/web-developer-at-buzzclan-4355374524</t>
+          <t>General software engineer role with no specific details</t>
+        </is>
+      </c>
+      <c r="H20" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-engineer-at-incline-4368479302</t>
         </is>
       </c>
       <c r="I20" s="2" t="inlineStr">
         <is>
-          <t>2026-02-04 15:43:30</t>
+          <t>2026-02-04 18:23:09</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
+          <t>Software Developer | Remote</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>Crossing Hurdles</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="F21" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="G21" s="2" t="inlineStr">
+        <is>
+          <t>Remote opportunity with flexible work arrangement</t>
+        </is>
+      </c>
+      <c r="H21" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-developer-remote-at-crossing-hurdles-4368211640</t>
+        </is>
+      </c>
+      <c r="I21" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Software Developer</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>nLeague</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>Nashville, TN</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>2025-11-26</t>
+        </is>
+      </c>
+      <c r="F22" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="G22" s="2" t="inlineStr">
+        <is>
+          <t>Software developer role in a specific location</t>
+        </is>
+      </c>
+      <c r="H22" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-developer-at-nleague-4339068108</t>
+        </is>
+      </c>
+      <c r="I22" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>Frontend JavaScript/TypeScript LLM - Remote</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>YO HR Consultancy</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-24</t>
+        </is>
+      </c>
+      <c r="F23" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G23" s="2" t="inlineStr">
+        <is>
+          <t>Remote frontend role with good technologies</t>
+        </is>
+      </c>
+      <c r="H23" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/frontend-javascript-typescript-llm-remote-at-yo-hr-consultancy-4355701088</t>
+        </is>
+      </c>
+      <c r="I23" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>Software Developer</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>CorSource</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="inlineStr">
+        <is>
+          <t>Portland, Oregon Metropolitan Area</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="F24" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="G24" s="2" t="inlineStr">
+        <is>
+          <t>Software developer role in a specific location with potential for growth</t>
+        </is>
+      </c>
+      <c r="H24" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-developer-at-corsource-4366038965</t>
+        </is>
+      </c>
+      <c r="I24" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>Front-End Developer- TX Locals</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="inlineStr">
+        <is>
+          <t>SIDRAM TECHNOLOGIES</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="inlineStr">
+        <is>
+          <t>Valley Spring, TX</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="F25" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G25" s="2" t="inlineStr">
+        <is>
+          <t>Front-end developer role with limited information</t>
+        </is>
+      </c>
+      <c r="H25" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/front-end-developer-tx-locals-at-sidram-technologies-4298228531</t>
+        </is>
+      </c>
+      <c r="I25" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>Software Engineer | $90/hr Remote</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>Crossing Hurdles</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-19</t>
+        </is>
+      </c>
+      <c r="F26" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G26" s="2" t="inlineStr">
+        <is>
+          <t>High paying remote software engineer role</t>
+        </is>
+      </c>
+      <c r="H26" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-engineer-%2490-hr-remote-at-crossing-hurdles-4359282892</t>
+        </is>
+      </c>
+      <c r="I26" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>Python Par</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="inlineStr">
+        <is>
+          <t>OVA.Work</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="inlineStr">
+        <is>
+          <t>Alpharetta, GA</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="F27" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G27" s="2" t="inlineStr">
+        <is>
+          <t>Python role with limited information but potential for growth</t>
+        </is>
+      </c>
+      <c r="H27" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/python-par-at-ova-work-4309339850</t>
+        </is>
+      </c>
+      <c r="I27" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>Software Engineer - Python (Advanced)</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>Alignerr</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="F28" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G28" s="2" t="inlineStr">
+        <is>
+          <t>Advanced role with specific technology, indicating a clear scope and potential for growth</t>
+        </is>
+      </c>
+      <c r="H28" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-engineer-python-advanced-at-alignerr-4366244522</t>
+        </is>
+      </c>
+      <c r="I28" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
           <t>Software Engineer | Remote</t>
         </is>
       </c>
-      <c r="B21" s="2" t="inlineStr">
+      <c r="B29" s="2" t="inlineStr">
         <is>
           <t>Crossing Hurdles</t>
         </is>
       </c>
-      <c r="C21" s="2" t="inlineStr">
+      <c r="C29" s="2" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="D21" s="2" t="inlineStr">
-        <is>
-          <t>Contract/Freelance</t>
-        </is>
-      </c>
-      <c r="E21" s="2" t="inlineStr">
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
         <is>
           <t>2026-02-02</t>
         </is>
       </c>
-      <c r="F21" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="G21" s="2" t="inlineStr">
-        <is>
-          <t>Reputable company, clear job title</t>
-        </is>
-      </c>
-      <c r="H21" s="4" t="inlineStr">
+      <c r="F29" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G29" s="2" t="inlineStr">
+        <is>
+          <t>Remote opportunity, offering flexibility and potentially a better work-life balance</t>
+        </is>
+      </c>
+      <c r="H29" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-engineer-remote-at-crossing-hurdles-4367885123</t>
+        </is>
+      </c>
+      <c r="I29" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>Full Stack Engineer</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>SIDRAM TECHNOLOGIES</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="inlineStr">
+        <is>
+          <t>Charlotte, NC</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>2025-09-30</t>
+        </is>
+      </c>
+      <c r="F30" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="G30" s="2" t="inlineStr">
+        <is>
+          <t>Full stack role with a specific location, indicating a clear scope and potential for collaboration</t>
+        </is>
+      </c>
+      <c r="H30" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/full-stack-engineer-at-sidram-technologies-4308476776</t>
+        </is>
+      </c>
+      <c r="I30" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>Application Engineer</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="inlineStr">
+        <is>
+          <t>Franklin Fitch</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="F31" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G31" s="2" t="inlineStr">
+        <is>
+          <t>Application engineer role with a reputable company, offering potential for growth and development</t>
+        </is>
+      </c>
+      <c r="H31" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/application-engineer-at-franklin-fitch-4366611035</t>
+        </is>
+      </c>
+      <c r="I31" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>Python web developer</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>OVA.Work</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="inlineStr">
+        <is>
+          <t>Alpharetta, GA</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="F32" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G32" s="2" t="inlineStr">
+        <is>
+          <t>Python web developer role with a specific location, indicating a clear scope and potential for collaboration</t>
+        </is>
+      </c>
+      <c r="H32" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/python-web-developer-at-ova-work-4309339840</t>
+        </is>
+      </c>
+      <c r="I32" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>Software Developer</t>
+        </is>
+      </c>
+      <c r="B33" s="2" t="inlineStr">
+        <is>
+          <t>PlanIT Group, LLC</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="inlineStr">
+        <is>
+          <t>Orlando, FL</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="F33" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="G33" s="2" t="inlineStr">
+        <is>
+          <t>Software developer role with a specific location, indicating a clear scope and potential for collaboration</t>
+        </is>
+      </c>
+      <c r="H33" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-developer-at-planit-group-llc-4239880773</t>
+        </is>
+      </c>
+      <c r="I33" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>Full Stack Engineer</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>Saransh Inc</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="inlineStr">
+        <is>
+          <t>Vienna, VA</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>2025-10-14</t>
+        </is>
+      </c>
+      <c r="F34" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G34" s="2" t="inlineStr">
+        <is>
+          <t>Full stack engineer role with a specific location, indicating a clear scope and potential for collaboration</t>
+        </is>
+      </c>
+      <c r="H34" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/full-stack-engineer-at-saransh-inc-4314693239</t>
+        </is>
+      </c>
+      <c r="I34" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>Web Engineer</t>
+        </is>
+      </c>
+      <c r="B35" s="2" t="inlineStr">
+        <is>
+          <t>OVA.Work</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="inlineStr">
+        <is>
+          <t>Alpharetta, GA</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="F35" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G35" s="2" t="inlineStr">
+        <is>
+          <t>Web engineer role with a specific location, indicating a clear scope and potential for collaboration</t>
+        </is>
+      </c>
+      <c r="H35" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/web-engineer-at-ova-work-4309345676</t>
+        </is>
+      </c>
+      <c r="I35" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>SDE 1- Backend</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="inlineStr">
+        <is>
+          <t>OVA.Work</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="inlineStr">
+        <is>
+          <t>Alpharetta, GA</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="F36" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="G36" s="2" t="inlineStr">
+        <is>
+          <t>Stable company, clear role definition</t>
+        </is>
+      </c>
+      <c r="H36" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/sde-1-backend-at-ova-work-4309337839</t>
+        </is>
+      </c>
+      <c r="I36" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="inlineStr">
+        <is>
+          <t>Python Web</t>
+        </is>
+      </c>
+      <c r="B37" s="2" t="inlineStr">
+        <is>
+          <t>OVA.Work</t>
+        </is>
+      </c>
+      <c r="C37" s="2" t="inlineStr">
+        <is>
+          <t>Alpharetta, GA</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="F37" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="G37" s="2" t="inlineStr">
+        <is>
+          <t>Specific technology mentioned, potential for growth</t>
+        </is>
+      </c>
+      <c r="H37" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/python-web-at-ova-work-4309349566</t>
+        </is>
+      </c>
+      <c r="I37" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="inlineStr">
+        <is>
+          <t>Website Developer – Freelance</t>
+        </is>
+      </c>
+      <c r="B38" s="2" t="inlineStr">
+        <is>
+          <t>Twine</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="F38" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G38" s="2" t="inlineStr">
+        <is>
+          <t>Freelance opportunity, flexible work arrangement</t>
+        </is>
+      </c>
+      <c r="H38" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/website-developer-%E2%80%93-freelance-at-twine-4356682524</t>
+        </is>
+      </c>
+      <c r="I38" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="inlineStr">
+        <is>
+          <t>Software Engineer (Python) | Remote</t>
+        </is>
+      </c>
+      <c r="B39" s="2" t="inlineStr">
+        <is>
+          <t>Crossing Hurdles</t>
+        </is>
+      </c>
+      <c r="C39" s="2" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="F39" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G39" s="2" t="inlineStr">
+        <is>
+          <t>Remote work option, specific technology mentioned</t>
+        </is>
+      </c>
+      <c r="H39" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-engineer-python-remote-at-crossing-hurdles-4368704822</t>
+        </is>
+      </c>
+      <c r="I39" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="inlineStr">
+        <is>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="B40" s="2" t="inlineStr">
+        <is>
+          <t>Motion Recruitment</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="inlineStr">
+        <is>
+          <t>Detroit Metropolitan Area</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="F40" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G40" s="2" t="inlineStr">
+        <is>
+          <t>Established company, potential for career advancement</t>
+        </is>
+      </c>
+      <c r="H40" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/web-developer-at-motion-recruitment-4366380465</t>
+        </is>
+      </c>
+      <c r="I40" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="inlineStr">
+        <is>
+          <t>Software Engineer | $80/hr | Remote</t>
+        </is>
+      </c>
+      <c r="B41" s="2" t="inlineStr">
+        <is>
+          <t>Crossing Hurdles</t>
+        </is>
+      </c>
+      <c r="C41" s="2" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-19</t>
+        </is>
+      </c>
+      <c r="F41" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G41" s="2" t="inlineStr">
+        <is>
+          <t>High hourly rate, remote work option, clear compensation</t>
+        </is>
+      </c>
+      <c r="H41" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-engineer-%2480-hr-remote-at-crossing-hurdles-4332552298</t>
+        </is>
+      </c>
+      <c r="I41" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="inlineStr">
+        <is>
+          <t>Software Engineer | $80/hr Remote</t>
+        </is>
+      </c>
+      <c r="B42" s="2" t="inlineStr">
+        <is>
+          <t>Crossing Hurdles</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="F42" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G42" s="2" t="inlineStr">
+        <is>
+          <t>High hourly rate, remote work option, clear compensation</t>
+        </is>
+      </c>
+      <c r="H42" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-engineer-%2480-hr-remote-at-crossing-hurdles-4368230010</t>
+        </is>
+      </c>
+      <c r="I42" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="B43" s="2" t="inlineStr">
+        <is>
+          <t>PlanIT Group, LLC</t>
+        </is>
+      </c>
+      <c r="C43" s="2" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="F43" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G43" s="2" t="inlineStr">
+        <is>
+          <t>National company, potential for career growth</t>
+        </is>
+      </c>
+      <c r="H43" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-engineer-at-planit-group-llc-4341020900</t>
+        </is>
+      </c>
+      <c r="I43" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="inlineStr">
+        <is>
+          <t>Web Application Developer</t>
+        </is>
+      </c>
+      <c r="B44" s="2" t="inlineStr">
+        <is>
+          <t>Vista Applied Solutions Group Inc</t>
+        </is>
+      </c>
+      <c r="C44" s="2" t="inlineStr">
+        <is>
+          <t>Sacramento, CA</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E44" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-21</t>
+        </is>
+      </c>
+      <c r="F44" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="G44" s="2" t="inlineStr">
+        <is>
+          <t>Specific technology mentioned, stable company</t>
+        </is>
+      </c>
+      <c r="H44" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/web-application-developer-at-vista-applied-solutions-group-inc-4328744179</t>
+        </is>
+      </c>
+      <c r="I44" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="inlineStr">
+        <is>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="B45" s="2" t="inlineStr">
+        <is>
+          <t>Kforce Inc</t>
+        </is>
+      </c>
+      <c r="C45" s="2" t="inlineStr">
+        <is>
+          <t>West Jordan, UT</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E45" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="F45" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G45" s="2" t="inlineStr">
+        <is>
+          <t>Established company, potential for career advancement</t>
+        </is>
+      </c>
+      <c r="H45" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/web-developer-at-kforce-inc-4367652104</t>
+        </is>
+      </c>
+      <c r="I45" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="inlineStr">
+        <is>
+          <t>React Developer</t>
+        </is>
+      </c>
+      <c r="B46" s="2" t="inlineStr">
+        <is>
+          <t>First Soft Solutions LLC</t>
+        </is>
+      </c>
+      <c r="C46" s="2" t="inlineStr">
+        <is>
+          <t>Fort Lauderdale, FL</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="inlineStr">
+        <is>
+          <t>2025-09-23</t>
+        </is>
+      </c>
+      <c r="F46" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="G46" s="2" t="inlineStr">
+        <is>
+          <t>Established company and specific location</t>
+        </is>
+      </c>
+      <c r="H46" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/react-developer-at-first-soft-solutions-llc-4304943915</t>
+        </is>
+      </c>
+      <c r="I46" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="inlineStr">
+        <is>
+          <t>Software Developer</t>
+        </is>
+      </c>
+      <c r="B47" s="2" t="inlineStr">
+        <is>
+          <t>PlanIT Group, LLC</t>
+        </is>
+      </c>
+      <c r="C47" s="2" t="inlineStr">
+        <is>
+          <t>Eagan, MN</t>
+        </is>
+      </c>
+      <c r="D47" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E47" s="2" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="F47" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="G47" s="2" t="inlineStr">
+        <is>
+          <t>Established company and specific location</t>
+        </is>
+      </c>
+      <c r="H47" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-developer-at-planit-group-llc-4224306166</t>
+        </is>
+      </c>
+      <c r="I47" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="inlineStr">
+        <is>
+          <t>Software Engineer | $80/hr Remote</t>
+        </is>
+      </c>
+      <c r="B48" s="2" t="inlineStr">
+        <is>
+          <t>Crossing Hurdles</t>
+        </is>
+      </c>
+      <c r="C48" s="2" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E48" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="F48" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G48" s="2" t="inlineStr">
+        <is>
+          <t>High hourly rate and remote work option</t>
+        </is>
+      </c>
+      <c r="H48" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-engineer-%2480-hr-remote-at-crossing-hurdles-4368700664</t>
+        </is>
+      </c>
+      <c r="I48" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="inlineStr">
+        <is>
+          <t>Software Engineer | Remote</t>
+        </is>
+      </c>
+      <c r="B49" s="2" t="inlineStr">
+        <is>
+          <t>Crossing Hurdles</t>
+        </is>
+      </c>
+      <c r="C49" s="2" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E49" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="F49" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G49" s="2" t="inlineStr">
+        <is>
+          <t>Remote work option and potential for good pay</t>
+        </is>
+      </c>
+      <c r="H49" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-engineer-remote-at-crossing-hurdles-4368210715</t>
+        </is>
+      </c>
+      <c r="I49" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="inlineStr">
+        <is>
+          <t>Freelance Web Developer – SaaS Remote</t>
+        </is>
+      </c>
+      <c r="B50" s="2" t="inlineStr">
+        <is>
+          <t>Twine</t>
+        </is>
+      </c>
+      <c r="C50" s="2" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E50" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-19</t>
+        </is>
+      </c>
+      <c r="F50" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G50" s="2" t="inlineStr">
+        <is>
+          <t>Freelance opportunity with remote work option and SaaS experience</t>
+        </is>
+      </c>
+      <c r="H50" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/freelance-web-developer-%E2%80%93-saas-remote-at-twine-4353884798</t>
+        </is>
+      </c>
+      <c r="I50" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="inlineStr">
+        <is>
+          <t>Software Engineer | Remote</t>
+        </is>
+      </c>
+      <c r="B51" s="2" t="inlineStr">
+        <is>
+          <t>Crossing Hurdles</t>
+        </is>
+      </c>
+      <c r="C51" s="2" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E51" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="F51" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G51" s="2" t="inlineStr">
+        <is>
+          <t>Remote work option and potential for good pay</t>
+        </is>
+      </c>
+      <c r="H51" s="2" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/jobs/view/software-engineer-remote-at-crossing-hurdles-4367826027</t>
         </is>
       </c>
-      <c r="I21" s="2" t="inlineStr">
-        <is>
-          <t>2026-02-04 15:43:30</t>
+      <c r="I51" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="inlineStr">
+        <is>
+          <t>Software Engineer | Remote</t>
+        </is>
+      </c>
+      <c r="B52" s="2" t="inlineStr">
+        <is>
+          <t>Crossing Hurdles</t>
+        </is>
+      </c>
+      <c r="C52" s="2" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E52" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="F52" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G52" s="2" t="inlineStr">
+        <is>
+          <t>Remote work option and potential for good pay</t>
+        </is>
+      </c>
+      <c r="H52" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-engineer-remote-at-crossing-hurdles-4368719262</t>
+        </is>
+      </c>
+      <c r="I52" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="B53" s="2" t="inlineStr">
+        <is>
+          <t>PlanIT Group, LLC</t>
+        </is>
+      </c>
+      <c r="C53" s="2" t="inlineStr">
+        <is>
+          <t>Orlando, FL</t>
+        </is>
+      </c>
+      <c r="D53" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E53" s="2" t="inlineStr">
+        <is>
+          <t>2025-11-27</t>
+        </is>
+      </c>
+      <c r="F53" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="G53" s="2" t="inlineStr">
+        <is>
+          <t>Established company and specific location</t>
+        </is>
+      </c>
+      <c r="H53" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-engineer-at-planit-group-llc-4339174284</t>
+        </is>
+      </c>
+      <c r="I53" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="B54" s="2" t="inlineStr">
+        <is>
+          <t>PlanIT Group, LLC</t>
+        </is>
+      </c>
+      <c r="C54" s="2" t="inlineStr">
+        <is>
+          <t>Orlando, FL</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E54" s="2" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="F54" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="G54" s="2" t="inlineStr">
+        <is>
+          <t>Established company and specific location</t>
+        </is>
+      </c>
+      <c r="H54" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-engineer-at-planit-group-llc-4310104379</t>
+        </is>
+      </c>
+      <c r="I54" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="inlineStr">
+        <is>
+          <t>Software Engineer, University Graduate</t>
+        </is>
+      </c>
+      <c r="B55" s="2" t="inlineStr">
+        <is>
+          <t>HeyGen</t>
+        </is>
+      </c>
+      <c r="C55" s="2" t="inlineStr">
+        <is>
+          <t>Palo Alto, CA</t>
+        </is>
+      </c>
+      <c r="D55" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E55" s="2" t="inlineStr">
+        <is>
+          <t>2025-12-30</t>
+        </is>
+      </c>
+      <c r="F55" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G55" s="2" t="inlineStr">
+        <is>
+          <t>Entry-level position at a reputable company</t>
+        </is>
+      </c>
+      <c r="H55" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-engineer-university-graduate-at-heygen-4355444896</t>
+        </is>
+      </c>
+      <c r="I55" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="inlineStr">
+        <is>
+          <t>Software Engineer | $80/hr Remote</t>
+        </is>
+      </c>
+      <c r="B56" s="2" t="inlineStr">
+        <is>
+          <t>Crossing Hurdles</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>Contract/Freelance</t>
+        </is>
+      </c>
+      <c r="E56" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="F56" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G56" s="2" t="inlineStr">
+        <is>
+          <t>High hourly rate and remote work option</t>
+        </is>
+      </c>
+      <c r="H56" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/software-engineer-%2480-hr-remote-at-crossing-hurdles-4368700664</t>
+        </is>
+      </c>
+      <c r="I56" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04 18:23:10</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1"/>
-  <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H3" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H4" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H5" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H6" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H7" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H8" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H9" r:id="rId8"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H10" r:id="rId9"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H11" r:id="rId10"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H12" r:id="rId11"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H13" r:id="rId12"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H14" r:id="rId13"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H15" r:id="rId14"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H16" r:id="rId15"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H17" r:id="rId16"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H18" r:id="rId17"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H19" r:id="rId18"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H20" r:id="rId19"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H21" r:id="rId20"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>